<commit_message>
add instructions & improve scripts
</commit_message>
<xml_diff>
--- a/data/template_metadata.xlsx
+++ b/data/template_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inrb\Documents\ebola-nord-kivu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inrb\Documents\ebola-nord-kivu\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEE7FFF-B39A-4F61-B854-3855960B643E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB5D4FC-44D6-4EA7-9A7B-22AD24B6EBB0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="870" yWindow="440" windowWidth="18230" windowHeight="9760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - `Table 1" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -282,11 +279,8 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -298,28 +292,13 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -328,13 +307,19 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1497,224 +1482,225 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.36328125" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="1" customWidth="1"/>
-    <col min="3" max="256" width="16.36328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.36328125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="21" style="9" customWidth="1"/>
+    <col min="3" max="256" width="16.36328125" style="9" customWidth="1"/>
+    <col min="257" max="16384" width="16.36328125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.399999999999999" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="32.4" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="15"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1">
-      <c r="A4" s="16"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" ht="20" customHeight="1">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1">
-      <c r="A14" s="16"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" ht="20" customHeight="1">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" ht="20" customHeight="1">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>

</xml_diff>